<commit_message>
Aeroport Fin modèle conceptuel de données
</commit_message>
<xml_diff>
--- a/03-Databases/Analyse/06-Videos/Exo_videos.xlsx
+++ b/03-Databases/Analyse/06-Videos/Exo_videos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arfpasso-my.sharepoint.com/personal/fbreton_arfp_asso_fr/Documents/Documents/DWWM_2409_BF/base de données/Exercices_Base_donnees/Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbreton\Documents\Git\DWWM_2409_BF\03-Databases\Analyse\06-Videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="8_{030BC2B9-737A-42F2-A15B-99F67C734DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33B36B55-F6BE-4C02-B44B-4101180DDCBA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E61569-6CCE-4CA3-B180-CE7D5CC52312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="1545" windowWidth="23745" windowHeight="12675" xr2:uid="{D7865FB9-1184-429A-8F61-05F58B90ADB0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D7865FB9-1184-429A-8F61-05F58B90ADB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>On pose une question pour chaque colonne de donnée :  Pour une valeur de cette donnée, existe-t-il une seule valeur de la donnée située en ligne ?</t>
   </si>
   <si>
-    <t>Exemple : Est-ce qu'il existe un seul client_id pour client_name ?</t>
-  </si>
-  <si>
     <t>client_id</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>client_firstname</t>
+  </si>
+  <si>
+    <t>Exemple : Est-ce qu'il existe un seul client_name pour client_id ?</t>
   </si>
 </sst>
 </file>
@@ -198,14 +198,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,10 +258,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,7 +598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I5" sqref="I5"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,24 +616,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -653,25 +649,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -684,12 +680,12 @@
     </row>
     <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -697,7 +693,7 @@
     </row>
     <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -705,7 +701,7 @@
     </row>
     <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -713,7 +709,7 @@
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -721,12 +717,12 @@
     </row>
     <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -734,7 +730,7 @@
     </row>
     <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -742,7 +738,7 @@
     </row>
     <row r="13" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -750,7 +746,7 @@
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -758,12 +754,12 @@
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -771,12 +767,12 @@
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -784,7 +780,7 @@
     </row>
     <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -795,7 +791,7 @@
     </row>
     <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -809,7 +805,7 @@
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -823,12 +819,12 @@
     </row>
     <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -836,7 +832,7 @@
     </row>
     <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -844,12 +840,12 @@
     </row>
     <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>